<commit_message>
updating specific and whole GE plots and metrics
</commit_message>
<xml_diff>
--- a/Data/specificGE_metricscalculation.xlsx
+++ b/Data/specificGE_metricscalculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcald\Documents\PhDThesis_Chapter4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C311F5C-9FFC-47A0-9994-72CC357FD681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5F482B-E404-42FA-8D74-35503C7797F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3F0E5D4A-E54B-40DA-95F3-4D9384949A20}"/>
+    <workbookView xWindow="20370" yWindow="-2175" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{3F0E5D4A-E54B-40DA-95F3-4D9384949A20}"/>
   </bookViews>
   <sheets>
     <sheet name="CR" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,12 +273,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -482,12 +476,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9806,7 +9800,7 @@
         <v>2.44</v>
       </c>
       <c r="Y128" s="2">
-        <f t="shared" ref="Y128:Y159" si="164">T128</f>
+        <f t="shared" ref="Y128" si="164">T128</f>
         <v>1.51</v>
       </c>
       <c r="Z128" s="2">
@@ -9824,7 +9818,7 @@
         <v>1.214311266722216</v>
       </c>
       <c r="AF128" s="2">
-        <f t="shared" ref="AF128:AF159" si="165">(AC128-Z128)/(LN(AC128/Z128))</f>
+        <f t="shared" ref="AF128" si="165">(AC128-Z128)/(LN(AC128/Z128))</f>
         <v>0.52290101981876691</v>
       </c>
     </row>
@@ -10314,7 +10308,7 @@
         <v>#NUM!</v>
       </c>
       <c r="AF135" s="19" t="e">
-        <f t="shared" ref="AF135:AF166" si="179">(AC135-Z135)/(LN(AC135/Z135))</f>
+        <f t="shared" ref="AF135" si="179">(AC135-Z135)/(LN(AC135/Z135))</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -10794,7 +10788,7 @@
         <v>2.68</v>
       </c>
       <c r="Y142" s="2">
-        <f t="shared" ref="Y142:Y183" si="187">T142</f>
+        <f t="shared" ref="Y142" si="187">T142</f>
         <v>2.2400000000000002</v>
       </c>
       <c r="Z142" s="2">
@@ -10812,7 +10806,7 @@
         <v>1.4833836174582649</v>
       </c>
       <c r="AF142" s="2">
-        <f t="shared" ref="AF142:AF183" si="188">(AC142-Z142)/(LN(AC142/Z142))</f>
+        <f t="shared" ref="AF142" si="188">(AC142-Z142)/(LN(AC142/Z142))</f>
         <v>0.16346172839254977</v>
       </c>
     </row>
@@ -11294,7 +11288,7 @@
         <v>1.4747975462020004</v>
       </c>
       <c r="AF149" s="2">
-        <f t="shared" ref="AF149:AF183" si="200">(AC149-Z149)/(LN(AC149/Z149))</f>
+        <f t="shared" ref="AF149" si="200">(AC149-Z149)/(LN(AC149/Z149))</f>
         <v>0.16251558470380162</v>
       </c>
     </row>
@@ -11766,7 +11760,7 @@
         <v>1.116992</v>
       </c>
       <c r="Y156" s="2">
-        <f t="shared" ref="Y156:Y183" si="207">T156</f>
+        <f t="shared" ref="Y156" si="207">T156</f>
         <v>0.41887199999999997</v>
       </c>
       <c r="Z156" s="2">
@@ -11784,7 +11778,7 @@
         <v>0.57587754748017761</v>
       </c>
       <c r="AF156" s="2">
-        <f t="shared" ref="AF156:AF183" si="208">(AC156-Z156)/(LN(AC156/Z156))</f>
+        <f t="shared" ref="AF156" si="208">(AC156-Z156)/(LN(AC156/Z156))</f>
         <v>0.1313368349985167</v>
       </c>
     </row>
@@ -12274,7 +12268,7 @@
         <v>0.45288155769557092</v>
       </c>
       <c r="AF163" s="2">
-        <f t="shared" ref="AF163:AF183" si="216">(AC163-Z163)/(LN(AC163/Z163))</f>
+        <f t="shared" ref="AF163" si="216">(AC163-Z163)/(LN(AC163/Z163))</f>
         <v>0.10328589936731607</v>
       </c>
     </row>
@@ -12754,7 +12748,7 @@
         <v>1.186804</v>
       </c>
       <c r="Y170" s="2">
-        <f t="shared" ref="Y170:Y183" si="223">T170</f>
+        <f t="shared" ref="Y170" si="223">T170</f>
         <v>0.94246200000000002</v>
       </c>
       <c r="Z170" s="2">
@@ -12772,7 +12766,7 @@
         <v>1.0920179951521176</v>
       </c>
       <c r="AF170" s="2">
-        <f t="shared" ref="AF170:AF183" si="224">(AC170-Z170)/(LN(AC170/Z170))</f>
+        <f t="shared" ref="AF170" si="224">(AC170-Z170)/(LN(AC170/Z170))</f>
         <v>0.14547495640513755</v>
       </c>
     </row>
@@ -13235,11 +13229,11 @@
         <v>1.6376774504566965E-2</v>
       </c>
       <c r="Q177" s="2">
-        <f t="shared" ref="Q177:Q183" si="229">(LN(V177)-LN(T177))/L177</f>
+        <f t="shared" ref="Q177:Q181" si="229">(LN(V177)-LN(T177))/L177</f>
         <v>1.9967511847944149E-2</v>
       </c>
       <c r="R177" s="2">
-        <f t="shared" ref="R177:R183" si="230">(LN(W177)-LN(T177))/L177</f>
+        <f t="shared" ref="R177:R181" si="230">(LN(W177)-LN(T177))/L177</f>
         <v>9.6051524421596774E-3</v>
       </c>
       <c r="T177" s="2">
@@ -13270,7 +13264,7 @@
         <v>1.1545262872975373</v>
       </c>
       <c r="AF177" s="2">
-        <f t="shared" ref="AF177:AF183" si="232">(AC177-Z177)/(LN(AC177/Z177))</f>
+        <f t="shared" ref="AF177" si="232">(AC177-Z177)/(LN(AC177/Z177))</f>
         <v>0.15380210038553302</v>
       </c>
     </row>
@@ -18505,7 +18499,7 @@
         <v>1</v>
       </c>
       <c r="D128" s="2">
-        <f t="shared" ref="D128:D159" si="63">I128*L128</f>
+        <f t="shared" ref="D128" si="63">I128*L128</f>
         <v>0.15814493998864881</v>
       </c>
       <c r="E128" s="2">
@@ -18768,7 +18762,7 @@
         <v>1</v>
       </c>
       <c r="D135" s="19" t="e">
-        <f t="shared" ref="D135:D166" si="67">I135*L135</f>
+        <f t="shared" ref="D135" si="67">I135*L135</f>
         <v>#NUM!</v>
       </c>
       <c r="E135" s="19" t="e">
@@ -19034,7 +19028,7 @@
         <v>1</v>
       </c>
       <c r="D142" s="2">
-        <f t="shared" ref="D142:D183" si="71">I142*L142</f>
+        <f t="shared" ref="D142" si="71">I142*L142</f>
         <v>1.5884221622612833</v>
       </c>
       <c r="E142" s="2">
@@ -19297,7 +19291,7 @@
         <v>1</v>
       </c>
       <c r="D149" s="2">
-        <f t="shared" ref="D149:D183" si="74">I149*L149</f>
+        <f t="shared" ref="D149" si="74">I149*L149</f>
         <v>2.6669155654440422</v>
       </c>
       <c r="E149" s="2">
@@ -19457,15 +19451,15 @@
         <v>0.79549169500006156</v>
       </c>
       <c r="E153" s="19">
-        <f t="shared" ref="E153:E183" si="75">J153*L153</f>
+        <f t="shared" ref="E153:E181" si="75">J153*L153</f>
         <v>99.436461875007694</v>
       </c>
       <c r="F153" s="19">
-        <f t="shared" ref="F153:F183" si="76">I153*M153</f>
+        <f t="shared" ref="F153:F181" si="76">I153*M153</f>
         <v>8.7659352480537731E-2</v>
       </c>
       <c r="G153" s="19">
-        <f t="shared" ref="G153:G183" si="77">J153*M153</f>
+        <f t="shared" ref="G153:G181" si="77">J153*M153</f>
         <v>10.957419060067217</v>
       </c>
       <c r="I153" s="20">
@@ -19561,7 +19555,7 @@
         <v>1</v>
       </c>
       <c r="D156" s="2">
-        <f t="shared" ref="D156:D183" si="80">I156*L156</f>
+        <f t="shared" ref="D156" si="80">I156*L156</f>
         <v>0.14466647273435893</v>
       </c>
       <c r="E156" s="2">
@@ -19825,7 +19819,7 @@
         <v>1</v>
       </c>
       <c r="D163" s="2">
-        <f t="shared" ref="D163:D183" si="83">I163*L163</f>
+        <f t="shared" ref="D163" si="83">I163*L163</f>
         <v>0.54498884521576596</v>
       </c>
       <c r="E163" s="2">
@@ -20090,7 +20084,7 @@
         <v>1</v>
       </c>
       <c r="D170" s="2">
-        <f t="shared" ref="D170:D183" si="86">I170*L170</f>
+        <f t="shared" ref="D170" si="86">I170*L170</f>
         <v>0.21787830640920317</v>
       </c>
       <c r="E170" s="2">
@@ -20355,7 +20349,7 @@
         <v>1</v>
       </c>
       <c r="D177" s="2">
-        <f t="shared" ref="D177:D183" si="89">I177*L177</f>
+        <f t="shared" ref="D177" si="89">I177*L177</f>
         <v>0.17273336057124511</v>
       </c>
       <c r="E177" s="2">
@@ -20618,7 +20612,7 @@
   <dimension ref="A1:J183"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20690,7 +20684,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">LN(G3/F3)</f>
+        <f>LN(G3/F3)</f>
         <v>-0.76546784213957142</v>
       </c>
       <c r="F3" s="2">
@@ -20714,7 +20708,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D3:D6" si="0">LN(G4/F4)</f>
         <v>-2.1517622032594619</v>
       </c>
       <c r="F4" s="2">
@@ -20880,7 +20874,7 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D10:D13" si="1">LN(G11/F11)</f>
+        <f t="shared" ref="D11:D13" si="1">LN(G11/F11)</f>
         <v>-0.3600027340314072</v>
       </c>
       <c r="F11" s="2">
@@ -21022,7 +21016,7 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D16:D20" si="2">LN(G17/F17)</f>
+        <f t="shared" ref="D17:D20" si="2">LN(G17/F17)</f>
         <v>-8.0042707673536495E-2</v>
       </c>
       <c r="F17" s="2">
@@ -21188,7 +21182,7 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D27" si="3">LN(G24/F24)</f>
+        <f t="shared" ref="D24:D26" si="3">LN(G24/F24)</f>
         <v>-0.48550781578170077</v>
       </c>
       <c r="F24" s="2">
@@ -22184,7 +22178,7 @@
         <v>2</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D69" si="9">LN(G66/F66)</f>
+        <f t="shared" ref="D66:D68" si="9">LN(G66/F66)</f>
         <v>-9.5310179804324768E-2</v>
       </c>
       <c r="F66" s="2">
@@ -23536,7 +23530,7 @@
         <v>3</v>
       </c>
       <c r="D123" s="37">
-        <f t="shared" ref="D122:D125" si="17">LN(G123/F123)</f>
+        <f t="shared" ref="D123:D125" si="17">LN(G123/F123)</f>
         <v>9.3090423066012035E-2</v>
       </c>
       <c r="F123" s="2">
@@ -24972,7 +24966,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C183" xr:uid="{FAF55A29-ECFE-4BB2-9D3C-EDA357ED9211}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
commit corrected lnR values and input data
</commit_message>
<xml_diff>
--- a/Data/specificGE_metricscalculation.xlsx
+++ b/Data/specificGE_metricscalculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcald\Documents\PhDThesis_Chapter4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5F482B-E404-42FA-8D74-35503C7797F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEE937C-B282-4EC9-BE7B-43783527A91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2175" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{3F0E5D4A-E54B-40DA-95F3-4D9384949A20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3F0E5D4A-E54B-40DA-95F3-4D9384949A20}"/>
   </bookViews>
   <sheets>
     <sheet name="CR" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CR!$A$1:$E$183</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EffectSize!$A$1:$C$183</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EffectSize!$A$1:$H$183</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IR!$A$1:$G$183</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="48">
   <si>
     <t>Treatment</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cnt_t24_cell.mL </t>
+  </si>
+  <si>
+    <t>lnRcorrect</t>
   </si>
 </sst>
 </file>
@@ -20612,7 +20615,7 @@
   <dimension ref="A1:J183"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20620,6 +20623,7 @@
     <col min="1" max="1" width="21.140625" style="23" customWidth="1"/>
     <col min="2" max="2" width="13" style="23" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="23"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="2"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
@@ -20637,6 +20641,9 @@
       <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F1" s="3" t="s">
         <v>28</v>
       </c>
@@ -20708,7 +20715,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D3:D6" si="0">LN(G4/F4)</f>
+        <f t="shared" ref="D4:D6" si="0">LN(G4/F4)</f>
         <v>-2.1517622032594619</v>
       </c>
       <c r="F4" s="2">
@@ -20783,6 +20790,10 @@
         <f>AVERAGE(D2:D6)</f>
         <v>-1.055634418591064</v>
       </c>
+      <c r="E7" s="33">
+        <f>LN(G7/F7)</f>
+        <v>-0.87082835779739776</v>
+      </c>
       <c r="F7" s="33">
         <f>AVERAGE(H2:H6)</f>
         <v>0.60038320000000001</v>
@@ -20949,6 +20960,10 @@
         <f>AVERAGE(D9:D11,D13)</f>
         <v>-0.21100687600483276</v>
       </c>
+      <c r="E14" s="34">
+        <f>LN(G14/F14)</f>
+        <v>-0.20585205420414873</v>
+      </c>
       <c r="F14" s="7">
         <f>AVERAGE(H9:H13)</f>
         <v>0.60038320000000001</v>
@@ -21115,6 +21130,10 @@
         <f>AVERAGE(D16:D19)</f>
         <v>-0.4002761690390525</v>
       </c>
+      <c r="E21" s="33">
+        <f>LN(G21/F21)</f>
+        <v>-0.36772478012531723</v>
+      </c>
       <c r="F21" s="33">
         <f>AVERAGE(H16:H20)</f>
         <v>0.52</v>
@@ -21281,6 +21300,10 @@
         <f>AVERAGE(D23:D27)</f>
         <v>-0.62728692328731772</v>
       </c>
+      <c r="E28" s="34">
+        <f>LN(G28/F28)</f>
+        <v>-0.59086833143952722</v>
+      </c>
       <c r="F28" s="34">
         <f>AVERAGE(H23:H27)</f>
         <v>0.52</v>
@@ -21447,6 +21470,10 @@
         <f>AVERAGE(D30:D33)</f>
         <v>-0.44190829476798632</v>
       </c>
+      <c r="E35" s="33">
+        <f>LN(G35/F35)</f>
+        <v>-0.36912240439195509</v>
+      </c>
       <c r="F35" s="5">
         <f>AVERAGE(H30:H34)</f>
         <v>7.4978087999999987</v>
@@ -21613,6 +21640,10 @@
         <f>AVERAGE(D38:D41)</f>
         <v>-0.43001891186719549</v>
       </c>
+      <c r="E42" s="34">
+        <f>LN(G42/F42)</f>
+        <v>-0.34582684178843304</v>
+      </c>
       <c r="F42" s="7">
         <f>AVERAGE(H37:H41)</f>
         <v>7.4978087999999987</v>
@@ -21779,6 +21810,10 @@
         <f>AVERAGE(D44:D48)</f>
         <v>-1.365869234140535</v>
       </c>
+      <c r="E49" s="33">
+        <f>LN(G49/F49)</f>
+        <v>-1.3083328196501787</v>
+      </c>
       <c r="F49" s="5">
         <f>AVERAGE(H44:H48)</f>
         <v>0.51660879999999998</v>
@@ -21945,6 +21980,10 @@
         <f>AVERAGE(D51,D53:D55)</f>
         <v>-0.86039295234316493</v>
       </c>
+      <c r="E56" s="34">
+        <f>LN(G56/F56)</f>
+        <v>-0.74871703171475612</v>
+      </c>
       <c r="F56" s="7">
         <f>AVERAGE(H51:H55)</f>
         <v>0.51660879999999998</v>
@@ -22111,6 +22150,10 @@
         <f>AVERAGE(D58,D60:D62)</f>
         <v>-0.36963846303844716</v>
       </c>
+      <c r="E63" s="33">
+        <f>LN(G63/F63)</f>
+        <v>-0.33950714031636675</v>
+      </c>
       <c r="F63" s="5">
         <f>AVERAGE(H58:H62)</f>
         <v>2.3037959999999997</v>
@@ -22277,6 +22320,10 @@
         <f>AVERAGE(D66:D69)</f>
         <v>-0.28485509251202479</v>
       </c>
+      <c r="E70" s="34">
+        <f>LN(G70/F70)</f>
+        <v>-0.2776317365982795</v>
+      </c>
       <c r="F70" s="7">
         <f>AVERAGE(H65:H69)</f>
         <v>2.3037959999999997</v>
@@ -22443,6 +22490,10 @@
         <f>AVERAGE(D72:D76)</f>
         <v>-0.54188193801522089</v>
       </c>
+      <c r="E77" s="33">
+        <f>LN(G77/F77)</f>
+        <v>-0.48550781578170077</v>
+      </c>
       <c r="F77" s="5">
         <f>AVERAGE(H72:H76)</f>
         <v>0.72604479999999993</v>
@@ -22609,6 +22660,10 @@
         <f>AVERAGE(D79:D83)</f>
         <v>-5.5549510961383261E-2</v>
       </c>
+      <c r="E84" s="34">
+        <f>LN(G84/F84)</f>
+        <v>1.904819497069463E-2</v>
+      </c>
       <c r="F84" s="7">
         <f>AVERAGE(H79:H83)</f>
         <v>0.72604479999999993</v>
@@ -22775,6 +22830,10 @@
         <f>AVERAGE(D86:D88,D90)</f>
         <v>-0.23850182948426668</v>
       </c>
+      <c r="E91" s="33">
+        <f>LN(G91/F91)</f>
+        <v>-0.19985599233344334</v>
+      </c>
       <c r="F91" s="5">
         <f>AVERAGE(H86:H90)</f>
         <v>0.46890959999999993</v>
@@ -22941,6 +23000,10 @@
         <f>AVERAGE(D93:D96)</f>
         <v>-0.41694344642493691</v>
       </c>
+      <c r="E98" s="34">
+        <f>LN(G98/F98)</f>
+        <v>-0.40052668779559453</v>
+      </c>
       <c r="F98" s="7">
         <f>AVERAGE(H93:H97)</f>
         <v>0.46890959999999993</v>
@@ -23107,6 +23170,10 @@
         <f>AVERAGE(D100:D104)</f>
         <v>-0.51585549071786108</v>
       </c>
+      <c r="E105" s="33">
+        <f>LN(G105/F105)</f>
+        <v>-0.5059356384717989</v>
+      </c>
       <c r="F105" s="5">
         <f>AVERAGE(H100:H104)</f>
         <v>0.94944320000000015</v>
@@ -23273,6 +23340,10 @@
         <f>AVERAGE(D108,D110:D111)</f>
         <v>-0.30748469974796089</v>
       </c>
+      <c r="E112" s="34">
+        <f>LN(G112/F112)</f>
+        <v>-0.30748469974796089</v>
+      </c>
       <c r="F112" s="7">
         <f>AVERAGE(H107:H111)</f>
         <v>0.94944320000000015</v>
@@ -23439,6 +23510,10 @@
         <f>AVERAGE(D116:D117)</f>
         <v>-0.4035354634391296</v>
       </c>
+      <c r="E119" s="33">
+        <f>LN(G119/F119)</f>
+        <v>-0.39938606203178212</v>
+      </c>
       <c r="F119" s="5">
         <f>AVERAGE(H114:H118)</f>
         <v>0.57245839999999992</v>
@@ -23605,6 +23680,10 @@
         <f>AVERAGE(D122:D125)</f>
         <v>-0.11274776098770942</v>
       </c>
+      <c r="E126" s="34">
+        <f>LN(G126/F126)</f>
+        <v>-8.9231133727942516E-2</v>
+      </c>
       <c r="F126" s="7">
         <f>AVERAGE(H121:H125)</f>
         <v>0.57245839999999992</v>
@@ -23771,6 +23850,10 @@
         <f>AVERAGE(D128:D132)</f>
         <v>-1.212988283868857</v>
       </c>
+      <c r="E133" s="33">
+        <f>LN(G133/F133)</f>
+        <v>-1.0004936354584093</v>
+      </c>
       <c r="F133" s="5">
         <f>AVERAGE(H128:H132)</f>
         <v>1.0878496</v>
@@ -23937,6 +24020,10 @@
         <f>AVERAGE(D137,D139)</f>
         <v>-1.3598579066839105</v>
       </c>
+      <c r="E140" s="34">
+        <f>LN(G140/F140)</f>
+        <v>-1.1367143553697008</v>
+      </c>
       <c r="F140" s="7">
         <f>AVERAGE(H135:H139)</f>
         <v>1.0878496</v>
@@ -24103,6 +24190,10 @@
         <f>AVERAGE(D142:D146)</f>
         <v>-1.1073811907481537</v>
       </c>
+      <c r="E147" s="33">
+        <f>LN(G147/F147)</f>
+        <v>-1.0797443305651635</v>
+      </c>
       <c r="F147" s="5">
         <f>AVERAGE(H142:H146)</f>
         <v>2.5717743999999998</v>
@@ -24269,6 +24360,10 @@
         <f>AVERAGE(D149:D152)</f>
         <v>-1.2465000917219389</v>
       </c>
+      <c r="E154" s="34">
+        <f>LN(G154/F154)</f>
+        <v>-1.2316396983327955</v>
+      </c>
       <c r="F154" s="7">
         <f>AVERAGE(H149:H153)</f>
         <v>2.5717743999999998</v>
@@ -24435,6 +24530,10 @@
         <f>AVERAGE(D156,D158:D160)</f>
         <v>-0.42815355656927134</v>
       </c>
+      <c r="E161" s="33">
+        <f>LN(G161/F161)</f>
+        <v>-0.41443377809092463</v>
+      </c>
       <c r="F161" s="5">
         <f>AVERAGE(H156:H160)</f>
         <v>0.9773679999999999</v>
@@ -24601,6 +24700,10 @@
         <f>AVERAGE(D163,D166:D167)</f>
         <v>-0.648636716351771</v>
       </c>
+      <c r="E168" s="34">
+        <f>LN(G168/F168)</f>
+        <v>-0.64662716492505246</v>
+      </c>
       <c r="F168" s="7">
         <f>AVERAGE(H163:H167)</f>
         <v>0.9773679999999999</v>
@@ -24767,6 +24870,10 @@
         <f>AVERAGE(D170,D173:D174)</f>
         <v>-0.7269902938644428</v>
       </c>
+      <c r="E175" s="33">
+        <f>LN(G175/F175)</f>
+        <v>-0.59700332000704315</v>
+      </c>
       <c r="F175" s="5">
         <f>AVERAGE(H170:H174)</f>
         <v>1.5219016000000001</v>
@@ -24933,6 +25040,10 @@
         <f>AVERAGE(D177:D181)</f>
         <v>-0.18647655550847367</v>
       </c>
+      <c r="E182" s="34">
+        <f>LN(G182/F182)</f>
+        <v>-0.18048837571229392</v>
+      </c>
       <c r="F182" s="7">
         <f>AVERAGE(H177:H181)</f>
         <v>1.5219016000000001</v>
@@ -24966,6 +25077,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H183" xr:uid="{FAF55A29-ECFE-4BB2-9D3C-EDA357ED9211}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>